<commit_message>
README for basic usage
</commit_message>
<xml_diff>
--- a/test/data/refactoring.xlsx
+++ b/test/data/refactoring.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devsisters\.julia\dev\XLSXasJSON\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maste\.julia\dev\XLSXasJSON\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB12463-4063-4B0B-9ADC-DD01AC1CC007}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="4365" windowWidth="21600" windowHeight="11835" activeTab="3"/>
+    <workbookView xWindow="735" yWindow="3375" windowWidth="21600" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="2" r:id="rId1"/>
@@ -22,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>d1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -183,58 +178,66 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>a.b.c.d.e.f</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a.b.c2(Int)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a.d.c.d.e.f.[1,Type]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a.d.c.d.e.f.[1,Amount]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a.d.c.d.e.f.[2,Type]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a.d.c.d.e.f.[2,Amount]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a.d.c.d.e.f.[2,Vec()]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>인셉션!!</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>100;200;300</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>후후</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이것도</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이런것;충분히;가능</t>
+    <t>Cake</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chocolate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Salt;100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ingredient</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b2(Int)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b3.[1,Type]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b3.[1,Amount]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b3.[2,Type]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b3.[2,Amount]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b3.[3,Type]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.b3.[3,Amount()]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fooood</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,11 +602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -670,7 +673,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -763,11 +766,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -842,63 +845,70 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="1">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="1">
-        <v>100</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="1">
-        <v>200</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>